<commit_message>
Set up ReadInput workflow
</commit_message>
<xml_diff>
--- a/Data/input.xlsx
+++ b/Data/input.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/230297338633d02e/Desktop/Facultate/Anul 4/Sem 1/RPA/OnlineProductSearchRPA/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="11_F25DC773A252ABDACC10482BC9DE568E5BDE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4CC02B2A-919B-4939-A657-F36D5EDA1C9D}"/>
+  <xr:revisionPtr revIDLastSave="31" documentId="11_F25DC773A252ABDACC10482BC9DE568E5BDE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{21BE1F37-355C-454D-8C14-19580BC545E1}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
   <si>
     <t>Keyword</t>
   </si>
@@ -34,6 +34,48 @@
   </si>
   <si>
     <t>Max price</t>
+  </si>
+  <si>
+    <t>tricou</t>
+  </si>
+  <si>
+    <t>Color</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>alb</t>
+  </si>
+  <si>
+    <t>barbati</t>
+  </si>
+  <si>
+    <t>rochie</t>
+  </si>
+  <si>
+    <t>femei</t>
+  </si>
+  <si>
+    <t>rosu</t>
+  </si>
+  <si>
+    <t>camasa</t>
+  </si>
+  <si>
+    <t>bleumarin</t>
+  </si>
+  <si>
+    <t>geaca</t>
+  </si>
+  <si>
+    <t>negru</t>
+  </si>
+  <si>
+    <t>hanorac</t>
+  </si>
+  <si>
+    <t>verde</t>
   </si>
 </sst>
 </file>
@@ -86,6 +128,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -351,15 +397,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -368,6 +414,97 @@
       </c>
       <c r="C1" t="s">
         <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>50</v>
+      </c>
+      <c r="C2">
+        <v>150</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3">
+        <v>300</v>
+      </c>
+      <c r="C3">
+        <v>700</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4">
+        <v>170</v>
+      </c>
+      <c r="C4">
+        <v>400</v>
+      </c>
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5">
+        <v>450</v>
+      </c>
+      <c r="C5">
+        <v>1200</v>
+      </c>
+      <c r="D5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6">
+        <v>250</v>
+      </c>
+      <c r="C6">
+        <v>500</v>
+      </c>
+      <c r="D6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add validations for input data
</commit_message>
<xml_diff>
--- a/Data/input.xlsx
+++ b/Data/input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/230297338633d02e/Desktop/Facultate/Anul 4/Sem 1/RPA/OnlineProductSearchRPA/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="31" documentId="11_F25DC773A252ABDACC10482BC9DE568E5BDE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{21BE1F37-355C-454D-8C14-19580BC545E1}"/>
+  <xr:revisionPtr revIDLastSave="42" documentId="11_F25DC773A252ABDACC10482BC9DE568E5BDE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C883E729-1F19-4004-885E-D396289611B1}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="705" yWindow="705" windowWidth="16200" windowHeight="9308" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Products" sheetId="1" r:id="rId1"/>
@@ -400,7 +400,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
SearchProducts workflow in progress
</commit_message>
<xml_diff>
--- a/Data/input.xlsx
+++ b/Data/input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/230297338633d02e/Desktop/Facultate/Anul 4/Sem 1/RPA/OnlineProductSearchRPA/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="42" documentId="11_F25DC773A252ABDACC10482BC9DE568E5BDE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C883E729-1F19-4004-885E-D396289611B1}"/>
+  <xr:revisionPtr revIDLastSave="43" documentId="11_F25DC773A252ABDACC10482BC9DE568E5BDE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{197A4903-8C8B-4E48-BD13-3A638D686DA7}"/>
   <bookViews>
     <workbookView xWindow="705" yWindow="705" windowWidth="16200" windowHeight="9308" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -66,9 +66,6 @@
     <t>bleumarin</t>
   </si>
   <si>
-    <t>geaca</t>
-  </si>
-  <si>
     <t>negru</t>
   </si>
   <si>
@@ -76,6 +73,9 @@
   </si>
   <si>
     <t>verde</t>
+  </si>
+  <si>
+    <t>blugi</t>
   </si>
 </sst>
 </file>
@@ -400,7 +400,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -475,7 +475,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B5">
         <v>450</v>
@@ -484,7 +484,7 @@
         <v>1200</v>
       </c>
       <c r="D5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E5" t="s">
         <v>9</v>
@@ -492,7 +492,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6">
         <v>250</v>
@@ -501,7 +501,7 @@
         <v>500</v>
       </c>
       <c r="D6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E6" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
SearchProducts workflow is done
</commit_message>
<xml_diff>
--- a/Data/input.xlsx
+++ b/Data/input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/230297338633d02e/Desktop/Facultate/Anul 4/Sem 1/RPA/OnlineProductSearchRPA/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="43" documentId="11_F25DC773A252ABDACC10482BC9DE568E5BDE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{197A4903-8C8B-4E48-BD13-3A638D686DA7}"/>
+  <xr:revisionPtr revIDLastSave="44" documentId="11_F25DC773A252ABDACC10482BC9DE568E5BDE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4476C3DD-42ED-4D39-8140-84E1C6C993C8}"/>
   <bookViews>
     <workbookView xWindow="705" yWindow="705" windowWidth="16200" windowHeight="9308" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -397,15 +397,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:N13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="J11" sqref="J11:N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -422,7 +422,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -439,7 +439,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -456,54 +456,54 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="J11" t="s">
         <v>11</v>
       </c>
-      <c r="B4">
+      <c r="K11">
         <v>170</v>
       </c>
-      <c r="C4">
+      <c r="L11">
         <v>400</v>
       </c>
-      <c r="D4" t="s">
+      <c r="M11" t="s">
         <v>12</v>
       </c>
-      <c r="E4" t="s">
+      <c r="N11" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="J12" t="s">
         <v>16</v>
       </c>
-      <c r="B5">
+      <c r="K12">
         <v>450</v>
       </c>
-      <c r="C5">
+      <c r="L12">
         <v>1200</v>
       </c>
-      <c r="D5" t="s">
+      <c r="M12" t="s">
         <v>13</v>
       </c>
-      <c r="E5" t="s">
+      <c r="N12" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A6" t="s">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="J13" t="s">
         <v>14</v>
       </c>
-      <c r="B6">
+      <c r="K13">
         <v>250</v>
       </c>
-      <c r="C6">
+      <c r="L13">
         <v>500</v>
       </c>
-      <c r="D6" t="s">
+      <c r="M13" t="s">
         <v>15</v>
       </c>
-      <c r="E6" t="s">
+      <c r="N13" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>